<commit_message>
MàJ des testsUnitaire/Intégration + Création des fichiers de code finale
</commit_message>
<xml_diff>
--- a/02 - Gestion de projet/SPER - INDICATEURS - RISQUES/SPER_PRI_PROJET-IEC61499_V1_1.xlsx
+++ b/02 - Gestion de projet/SPER - INDICATEURS - RISQUES/SPER_PRI_PROJET-IEC61499_V1_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damienlorigeon/Documents/Polytech/5A/PRI/PRI-IEC61499-UniversalAutomation/02 - Gestion de projet/SPER - INDICATEURS - RISQUES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330680CD-CADF-FF41-AD3D-EE6B63681C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA534FE3-EA3B-4748-B231-9752DB6AA72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="16120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1880" windowWidth="28800" windowHeight="16120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthèse" sheetId="6" r:id="rId1"/>
@@ -630,336 +630,6 @@
   </cellStyles>
   <dxfs count="267">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7"/>
@@ -3378,6 +3048,32 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -3386,6 +3082,32 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3446,6 +3168,24 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -3471,6 +3211,32 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -3492,6 +3258,32 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3549,6 +3341,32 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3572,6 +3390,32 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3627,29 +3471,16 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3705,8 +3536,35 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3727,8 +3585,32 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3788,6 +3670,38 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3803,6 +3717,92 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -9675,111 +9675,111 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2E5B1876-2265-BD45-A1E2-F3FC886EA92A}" name="Novembre4" displayName="Novembre4" ref="B1:N31" totalsRowCount="1" headerRowDxfId="182" dataDxfId="180" headerRowBorderDxfId="181" tableBorderDxfId="179">
   <autoFilter ref="B1:N30" xr:uid="{2E5B1876-2265-BD45-A1E2-F3FC886EA92A}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{0BEA9DBC-9CC5-9E40-9C80-1F5698C0B8D7}" name="Tâche" totalsRowLabel="Total" dataDxfId="178" totalsRowDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{9780AF96-1A55-FD49-89CF-0C4EA8E61EA4}" name="Qui" dataDxfId="177" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{335BC6E3-0BCE-984D-A41E-51285FE6B047}" name="Charge Initiale (h)" totalsRowFunction="sum" dataDxfId="176" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{CDC0537A-9906-324A-8BBC-119335655680}" name="TPS Période(h)" totalsRowFunction="sum" dataDxfId="175" totalsRowDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{7AFAC50D-B2FD-B044-959B-6CD052C5451D}" name="TPS Cumul (h)" totalsRowFunction="sum" dataDxfId="174" totalsRowDxfId="8">
+    <tableColumn id="1" xr3:uid="{0BEA9DBC-9CC5-9E40-9C80-1F5698C0B8D7}" name="Tâche" totalsRowLabel="Total" dataDxfId="178" totalsRowDxfId="177"/>
+    <tableColumn id="11" xr3:uid="{9780AF96-1A55-FD49-89CF-0C4EA8E61EA4}" name="Qui" dataDxfId="176" totalsRowDxfId="175"/>
+    <tableColumn id="2" xr3:uid="{335BC6E3-0BCE-984D-A41E-51285FE6B047}" name="Charge Initiale (h)" totalsRowFunction="sum" dataDxfId="174" totalsRowDxfId="173"/>
+    <tableColumn id="3" xr3:uid="{CDC0537A-9906-324A-8BBC-119335655680}" name="TPS Période(h)" totalsRowFunction="sum" dataDxfId="172" totalsRowDxfId="171"/>
+    <tableColumn id="10" xr3:uid="{7AFAC50D-B2FD-B044-959B-6CD052C5451D}" name="TPS Cumul (h)" totalsRowFunction="sum" dataDxfId="170" totalsRowDxfId="169">
       <calculatedColumnFormula>Novembre4[[#This Row],[TPS Période(h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{164BBD2F-B98A-F144-9B3D-96906D36133F}" name="Reste à passer (h) " totalsRowFunction="sum" dataDxfId="173" totalsRowDxfId="7">
+    <tableColumn id="4" xr3:uid="{164BBD2F-B98A-F144-9B3D-96906D36133F}" name="Reste à passer (h) " totalsRowFunction="sum" dataDxfId="168" totalsRowDxfId="167">
       <calculatedColumnFormula>IF(N2="Non",MAX(Novembre4[[#This Row],[Charge Initiale (h)]]-Novembre4[[#This Row],[TPS Cumul (h)]],0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5E978354-8A8D-9A49-B9B4-F86596EFCE20}" name="CR (h)" totalsRowFunction="sum" dataDxfId="172" totalsRowDxfId="6">
+    <tableColumn id="5" xr3:uid="{5E978354-8A8D-9A49-B9B4-F86596EFCE20}" name="CR (h)" totalsRowFunction="sum" dataDxfId="166" totalsRowDxfId="165">
       <calculatedColumnFormula>Novembre4[[#This Row],[TPS Cumul (h)]]+Novembre4[[#This Row],[Reste à passer (h) ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E6CCE8E7-7D0C-A844-B95B-E88C22C46F4C}" name=" Ecart de charge (h)" totalsRowFunction="sum" dataDxfId="171" totalsRowDxfId="5">
+    <tableColumn id="6" xr3:uid="{E6CCE8E7-7D0C-A844-B95B-E88C22C46F4C}" name=" Ecart de charge (h)" totalsRowFunction="sum" dataDxfId="164" totalsRowDxfId="163">
       <calculatedColumnFormula>Novembre4[[#This Row],[CR (h)]] - Novembre4[[#This Row],[Charge Initiale (h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A69DCF95-9FB0-BE44-83F6-2778CEA77527}" name="Prix de revien unitaire(€)" totalsRowFunction="sum" dataDxfId="170" totalsRowDxfId="4">
+    <tableColumn id="7" xr3:uid="{A69DCF95-9FB0-BE44-83F6-2778CEA77527}" name="Prix de revien unitaire(€)" totalsRowFunction="sum" dataDxfId="162" totalsRowDxfId="161">
       <calculatedColumnFormula>IF(Novembre4[[#This Row],[Qui]]="Chef de projet","68",IF(Novembre4[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Novembre4[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Novembre4[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Novembre4[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{AF94DA91-71DE-4146-A3E8-C2AA58475207}" name="Coût Initial (€)" totalsRowFunction="sum" dataDxfId="169" totalsRowDxfId="3">
+    <tableColumn id="9" xr3:uid="{AF94DA91-71DE-4146-A3E8-C2AA58475207}" name="Coût Initial (€)" totalsRowFunction="sum" dataDxfId="160" totalsRowDxfId="159">
       <calculatedColumnFormula>IF(Novembre4[[#This Row],[TPS Cumul (h)]]&gt;0,Novembre4[[#This Row],[Charge Initiale (h)]]*Novembre4[[#This Row],[Prix de revien unitaire(€)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{384254D1-68E7-064F-8846-E5FC260547DC}" name="Coût Révisé (€)" totalsRowFunction="sum" dataDxfId="168" totalsRowDxfId="2">
+    <tableColumn id="8" xr3:uid="{384254D1-68E7-064F-8846-E5FC260547DC}" name="Coût Révisé (€)" totalsRowFunction="sum" dataDxfId="158" totalsRowDxfId="157">
       <calculatedColumnFormula>Novembre4[[#This Row],[CR (h)]]*Novembre4[[#This Row],[Prix de revien unitaire(€)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B3E7A0DA-393A-1A40-B73A-5ED2C080324C}" name="Coût Réel" totalsRowFunction="sum" dataDxfId="167" totalsRowDxfId="1">
+    <tableColumn id="12" xr3:uid="{B3E7A0DA-393A-1A40-B73A-5ED2C080324C}" name="Coût Réel" totalsRowFunction="sum" dataDxfId="156" totalsRowDxfId="155">
       <calculatedColumnFormula>Novembre4[[#This Row],[Prix de revien unitaire(€)]]*Novembre4[[#This Row],[TPS Cumul (h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3B42FE61-A79A-1B42-9435-B1E1C2EF680D}" name="Validation" dataDxfId="166" totalsRowDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{3B42FE61-A79A-1B42-9435-B1E1C2EF680D}" name="Validation" dataDxfId="154" totalsRowDxfId="153"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ABE6262C-FB6F-0A48-8368-139703B54F9D}" name="Novembre5" displayName="Novembre5" ref="B1:N31" totalsRowCount="1" headerRowDxfId="165" dataDxfId="163" headerRowBorderDxfId="164" tableBorderDxfId="162">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ABE6262C-FB6F-0A48-8368-139703B54F9D}" name="Novembre5" displayName="Novembre5" ref="B1:N31" totalsRowCount="1" headerRowDxfId="152" dataDxfId="150" headerRowBorderDxfId="151" tableBorderDxfId="149">
   <autoFilter ref="B1:N30" xr:uid="{ABE6262C-FB6F-0A48-8368-139703B54F9D}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C82A2965-B734-864C-A7C8-5D159DD6FACD}" name="Tâche" totalsRowLabel="Total" dataDxfId="161" totalsRowDxfId="160"/>
-    <tableColumn id="11" xr3:uid="{8E763832-AB8D-7944-A00F-54B7A99185D0}" name="Qui" dataDxfId="159" totalsRowDxfId="158"/>
-    <tableColumn id="2" xr3:uid="{33C7B5F8-FEE3-4640-B8F0-978D64245C91}" name="Charge Initiale (h)" totalsRowFunction="sum" dataDxfId="157" totalsRowDxfId="156"/>
-    <tableColumn id="3" xr3:uid="{B993F1E8-6C38-5E4A-BC55-A4C0F126E3DC}" name="TPS Période(h)" totalsRowFunction="sum" dataDxfId="155" totalsRowDxfId="154"/>
-    <tableColumn id="10" xr3:uid="{99F8DCF5-4000-DC42-BD02-8D9C8D84FC8D}" name="TPS Cumul (h)" totalsRowFunction="sum" dataDxfId="153" totalsRowDxfId="152">
+    <tableColumn id="1" xr3:uid="{C82A2965-B734-864C-A7C8-5D159DD6FACD}" name="Tâche" totalsRowLabel="Total" dataDxfId="148" totalsRowDxfId="147"/>
+    <tableColumn id="11" xr3:uid="{8E763832-AB8D-7944-A00F-54B7A99185D0}" name="Qui" dataDxfId="146" totalsRowDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{33C7B5F8-FEE3-4640-B8F0-978D64245C91}" name="Charge Initiale (h)" totalsRowFunction="sum" dataDxfId="144" totalsRowDxfId="143"/>
+    <tableColumn id="3" xr3:uid="{B993F1E8-6C38-5E4A-BC55-A4C0F126E3DC}" name="TPS Période(h)" totalsRowFunction="sum" dataDxfId="142" totalsRowDxfId="141"/>
+    <tableColumn id="10" xr3:uid="{99F8DCF5-4000-DC42-BD02-8D9C8D84FC8D}" name="TPS Cumul (h)" totalsRowFunction="sum" dataDxfId="140" totalsRowDxfId="139">
       <calculatedColumnFormula>Novembre5[[#This Row],[TPS Période(h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{92651564-1D3D-4340-BCB2-78C454BA2458}" name="Reste à passer (h) " totalsRowFunction="sum" dataDxfId="151" totalsRowDxfId="150">
+    <tableColumn id="4" xr3:uid="{92651564-1D3D-4340-BCB2-78C454BA2458}" name="Reste à passer (h) " totalsRowFunction="sum" dataDxfId="138" totalsRowDxfId="137">
       <calculatedColumnFormula>IF(N2="Non",MAX(Novembre5[[#This Row],[Charge Initiale (h)]]-Novembre5[[#This Row],[TPS Cumul (h)]],0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{40E135BC-65DC-8447-A30D-B6FB19297FA0}" name="CR (h)" totalsRowFunction="sum" dataDxfId="149" totalsRowDxfId="148">
+    <tableColumn id="5" xr3:uid="{40E135BC-65DC-8447-A30D-B6FB19297FA0}" name="CR (h)" totalsRowFunction="sum" dataDxfId="136" totalsRowDxfId="135">
       <calculatedColumnFormula>Novembre5[[#This Row],[TPS Cumul (h)]]+Novembre5[[#This Row],[Reste à passer (h) ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D11484C2-48BE-744A-9ACE-92B10D764EAB}" name=" Ecart de charge (h)" totalsRowFunction="sum" dataDxfId="147" totalsRowDxfId="146">
+    <tableColumn id="6" xr3:uid="{D11484C2-48BE-744A-9ACE-92B10D764EAB}" name=" Ecart de charge (h)" totalsRowFunction="sum" dataDxfId="134" totalsRowDxfId="133">
       <calculatedColumnFormula>Novembre5[[#This Row],[CR (h)]] - Novembre5[[#This Row],[Charge Initiale (h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4F2675EE-1760-9241-99E6-58A883367A31}" name="Prix de revien unitaire(€)" totalsRowFunction="sum" dataDxfId="145" totalsRowDxfId="144">
+    <tableColumn id="7" xr3:uid="{4F2675EE-1760-9241-99E6-58A883367A31}" name="Prix de revien unitaire(€)" totalsRowFunction="sum" dataDxfId="132" totalsRowDxfId="131">
       <calculatedColumnFormula>IF(Novembre5[[#This Row],[Qui]]="Chef de projet","68",IF(Novembre5[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Novembre5[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Novembre5[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Novembre5[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C846DFA2-65F6-CB4E-AEEC-22FA87C181FD}" name="Coût Initial (€)" totalsRowFunction="sum" dataDxfId="143" totalsRowDxfId="142">
+    <tableColumn id="9" xr3:uid="{C846DFA2-65F6-CB4E-AEEC-22FA87C181FD}" name="Coût Initial (€)" totalsRowFunction="sum" dataDxfId="130" totalsRowDxfId="129">
       <calculatedColumnFormula>IF(Novembre5[[#This Row],[TPS Cumul (h)]]&gt;0,Novembre5[[#This Row],[Charge Initiale (h)]]*Novembre5[[#This Row],[Prix de revien unitaire(€)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{F615F4B1-B5A8-2746-8227-0CBAAE52522B}" name="Coût Révisé (€)" totalsRowFunction="sum" dataDxfId="141" totalsRowDxfId="140">
+    <tableColumn id="8" xr3:uid="{F615F4B1-B5A8-2746-8227-0CBAAE52522B}" name="Coût Révisé (€)" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127">
       <calculatedColumnFormula>Novembre5[[#This Row],[CR (h)]]*Novembre5[[#This Row],[Prix de revien unitaire(€)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5FBCBCC7-AD98-BC48-8440-359658FCB0DD}" name="Coût Réel" totalsRowFunction="sum" dataDxfId="139" totalsRowDxfId="138">
+    <tableColumn id="12" xr3:uid="{5FBCBCC7-AD98-BC48-8440-359658FCB0DD}" name="Coût Réel" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125">
       <calculatedColumnFormula>Novembre5[[#This Row],[Prix de revien unitaire(€)]]*Novembre5[[#This Row],[TPS Cumul (h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D42F1B05-0748-A14D-8682-B7BC483D041E}" name="Validation" dataDxfId="137" totalsRowDxfId="136"/>
+    <tableColumn id="13" xr3:uid="{D42F1B05-0748-A14D-8682-B7BC483D041E}" name="Validation" dataDxfId="124" totalsRowDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CED7DF76-F011-A34B-BE70-E4BFC169CAA0}" name="Novembre6" displayName="Novembre6" ref="B1:N31" totalsRowCount="1" headerRowDxfId="135" dataDxfId="133" headerRowBorderDxfId="134" tableBorderDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CED7DF76-F011-A34B-BE70-E4BFC169CAA0}" name="Novembre6" displayName="Novembre6" ref="B1:N31" totalsRowCount="1" headerRowDxfId="122" dataDxfId="120" headerRowBorderDxfId="121" tableBorderDxfId="119">
   <autoFilter ref="B1:N30" xr:uid="{CED7DF76-F011-A34B-BE70-E4BFC169CAA0}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F4C7F033-A2F3-EA47-8E19-AB45414F742D}" name="Tâche" totalsRowLabel="Total" dataDxfId="131" totalsRowDxfId="130"/>
-    <tableColumn id="11" xr3:uid="{4DC72074-8A80-E04A-94A7-D76D9FBFD651}" name="Qui" dataDxfId="129" totalsRowDxfId="128"/>
-    <tableColumn id="2" xr3:uid="{C9D9F993-5CDB-7C4E-8D34-E1930E8546E3}" name="Charge Initiale (h)" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="126"/>
-    <tableColumn id="3" xr3:uid="{5B4319EC-5196-334D-8424-BA3D801B016F}" name="TPS Période(h)" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="124"/>
-    <tableColumn id="10" xr3:uid="{DF120DB6-1073-2C44-B926-AF98301A0CB3}" name="TPS Cumul (h)" totalsRowFunction="sum" dataDxfId="123" totalsRowDxfId="122">
+    <tableColumn id="1" xr3:uid="{F4C7F033-A2F3-EA47-8E19-AB45414F742D}" name="Tâche" totalsRowLabel="Total" dataDxfId="118" totalsRowDxfId="117"/>
+    <tableColumn id="11" xr3:uid="{4DC72074-8A80-E04A-94A7-D76D9FBFD651}" name="Qui" dataDxfId="116" totalsRowDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{C9D9F993-5CDB-7C4E-8D34-E1930E8546E3}" name="Charge Initiale (h)" totalsRowFunction="sum" dataDxfId="114" totalsRowDxfId="113"/>
+    <tableColumn id="3" xr3:uid="{5B4319EC-5196-334D-8424-BA3D801B016F}" name="TPS Période(h)" totalsRowFunction="sum" dataDxfId="112" totalsRowDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{DF120DB6-1073-2C44-B926-AF98301A0CB3}" name="TPS Cumul (h)" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="109">
       <calculatedColumnFormula>Novembre6[[#This Row],[TPS Période(h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CCB8E0BA-5622-C04C-AEED-45316203FDAD}" name="Reste à passer (h) " totalsRowFunction="sum" dataDxfId="121" totalsRowDxfId="120">
+    <tableColumn id="4" xr3:uid="{CCB8E0BA-5622-C04C-AEED-45316203FDAD}" name="Reste à passer (h) " totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="107">
       <calculatedColumnFormula>IF(N2="Non",MAX(Novembre6[[#This Row],[Charge Initiale (h)]]-Novembre6[[#This Row],[TPS Cumul (h)]],0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BD6EB6B5-983C-2E40-9F3A-B72750EE4EEC}" name="CR (h)" totalsRowFunction="sum" dataDxfId="119" totalsRowDxfId="118">
+    <tableColumn id="5" xr3:uid="{BD6EB6B5-983C-2E40-9F3A-B72750EE4EEC}" name="CR (h)" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="105">
       <calculatedColumnFormula>Novembre6[[#This Row],[TPS Cumul (h)]]+Novembre6[[#This Row],[Reste à passer (h) ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B300E6E0-2946-B944-9E78-7CE701F1BB8B}" name=" Ecart de charge (h)" totalsRowFunction="sum" dataDxfId="117" totalsRowDxfId="116">
+    <tableColumn id="6" xr3:uid="{B300E6E0-2946-B944-9E78-7CE701F1BB8B}" name=" Ecart de charge (h)" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="103">
       <calculatedColumnFormula>Novembre6[[#This Row],[CR (h)]] - Novembre6[[#This Row],[Charge Initiale (h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{40D8ADBD-415E-A54E-8E97-46E92B655B5B}" name="Prix de revien unitaire(€)" totalsRowFunction="sum" dataDxfId="115" totalsRowDxfId="114">
+    <tableColumn id="7" xr3:uid="{40D8ADBD-415E-A54E-8E97-46E92B655B5B}" name="Prix de revien unitaire(€)" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="101">
       <calculatedColumnFormula>IF(Novembre6[[#This Row],[Qui]]="Chef de projet","68",IF(Novembre6[[#This Row],[Qui]]="Ingénieur Electronique","32",IF(Novembre6[[#This Row],[Qui]]="Ingénieur qualité","36",IF(Novembre6[[#This Row],[Qui]]="Ingénieur Développement",30,IF(Novembre6[[#This Row],[Qui]]="Ingénieur Mécanique",34,"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0CC9BD66-F210-434E-98CD-05ED1716A1B5}" name="Coût Initial (€)" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112">
+    <tableColumn id="9" xr3:uid="{0CC9BD66-F210-434E-98CD-05ED1716A1B5}" name="Coût Initial (€)" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="99">
       <calculatedColumnFormula>IF(Novembre6[[#This Row],[TPS Cumul (h)]]&gt;0,Novembre6[[#This Row],[Charge Initiale (h)]]*Novembre6[[#This Row],[Prix de revien unitaire(€)]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{794993DB-2332-6C44-A439-A71039BC33A7}" name="Coût Révisé (€)" totalsRowFunction="sum" dataDxfId="111" totalsRowDxfId="110">
+    <tableColumn id="8" xr3:uid="{794993DB-2332-6C44-A439-A71039BC33A7}" name="Coût Révisé (€)" totalsRowFunction="sum" dataDxfId="98" totalsRowDxfId="97">
       <calculatedColumnFormula>Novembre6[[#This Row],[CR (h)]]*Novembre6[[#This Row],[Prix de revien unitaire(€)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{3F7AF828-7575-3649-8853-9C643EB6F906}" name="Coût Réel" totalsRowFunction="sum" dataDxfId="109" totalsRowDxfId="108">
+    <tableColumn id="12" xr3:uid="{3F7AF828-7575-3649-8853-9C643EB6F906}" name="Coût Réel" totalsRowFunction="sum" dataDxfId="96" totalsRowDxfId="95">
       <calculatedColumnFormula>Novembre6[[#This Row],[Prix de revien unitaire(€)]]*Novembre6[[#This Row],[TPS Cumul (h)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{ABCD7A7A-10F1-BE4B-9DB2-BF175D33097D}" name="Validation" dataDxfId="107" totalsRowDxfId="106"/>
+    <tableColumn id="13" xr3:uid="{ABCD7A7A-10F1-BE4B-9DB2-BF175D33097D}" name="Validation" dataDxfId="94" totalsRowDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11983,17 +11983,17 @@
     <mergeCell ref="A24:A25"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:E2">
-    <cfRule type="expression" dxfId="105" priority="78">
+    <cfRule type="expression" dxfId="92" priority="78">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M30">
-    <cfRule type="expression" dxfId="104" priority="6">
+    <cfRule type="expression" dxfId="91" priority="6">
       <formula>$F3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:M2">
-    <cfRule type="expression" dxfId="103" priority="1">
+    <cfRule type="expression" dxfId="90" priority="1">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13621,12 +13621,12 @@
     <mergeCell ref="A24:A25"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C30 E2:M30">
-    <cfRule type="expression" dxfId="102" priority="48">
+    <cfRule type="expression" dxfId="89" priority="48">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D30">
-    <cfRule type="expression" dxfId="101" priority="7">
+    <cfRule type="expression" dxfId="88" priority="7">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15275,98 +15275,98 @@
     <mergeCell ref="A24:A25"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3 D2:D30">
-    <cfRule type="expression" dxfId="100" priority="8">
+    <cfRule type="expression" dxfId="87" priority="8">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B9">
-    <cfRule type="expression" dxfId="99" priority="11">
+    <cfRule type="expression" dxfId="86" priority="11">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="98" priority="12">
+    <cfRule type="expression" dxfId="85" priority="12">
       <formula>$F4&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="expression" dxfId="97" priority="21">
+    <cfRule type="expression" dxfId="84" priority="21">
       <formula>$F12&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="96" priority="20">
+    <cfRule type="expression" dxfId="83" priority="20">
       <formula>$F13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="95" priority="15">
+    <cfRule type="expression" dxfId="82" priority="15">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B13">
-    <cfRule type="expression" dxfId="94" priority="14">
+    <cfRule type="expression" dxfId="81" priority="14">
       <formula>$F15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="expression" dxfId="93" priority="9">
+    <cfRule type="expression" dxfId="80" priority="9">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B28">
-    <cfRule type="expression" dxfId="92" priority="4">
+    <cfRule type="expression" dxfId="79" priority="4">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 B23:B26 B28 C2:C30 F2:M30">
-    <cfRule type="expression" dxfId="91" priority="16">
+    <cfRule type="expression" dxfId="78" priority="16">
       <formula>$N2="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="90" priority="18">
+    <cfRule type="expression" dxfId="77" priority="18">
       <formula>$N18="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="19">
+    <cfRule type="expression" dxfId="76" priority="19">
       <formula>$F18&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B28">
-    <cfRule type="expression" dxfId="88" priority="24">
+    <cfRule type="expression" dxfId="75" priority="24">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="25">
+    <cfRule type="expression" dxfId="74" priority="25">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="86" priority="22">
+    <cfRule type="expression" dxfId="73" priority="22">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="23">
+    <cfRule type="expression" dxfId="72" priority="23">
       <formula>#REF!&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="30">
+    <cfRule type="expression" dxfId="71" priority="30">
       <formula>$N29="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="31">
+    <cfRule type="expression" dxfId="70" priority="31">
       <formula>$F29&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="32">
+    <cfRule type="expression" dxfId="69" priority="32">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="33">
+    <cfRule type="expression" dxfId="68" priority="33">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C30 F2:M30 B21 B23:B26 B28">
-    <cfRule type="expression" dxfId="80" priority="17">
+    <cfRule type="expression" dxfId="67" priority="17">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="expression" dxfId="79" priority="1">
+    <cfRule type="expression" dxfId="66" priority="1">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17098,98 +17098,98 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3 D2:D30">
-    <cfRule type="expression" dxfId="78" priority="3">
+    <cfRule type="expression" dxfId="65" priority="3">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B9">
-    <cfRule type="expression" dxfId="77" priority="5">
+    <cfRule type="expression" dxfId="64" priority="5">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="76" priority="6">
+    <cfRule type="expression" dxfId="63" priority="6">
       <formula>$F4&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="expression" dxfId="75" priority="14">
+    <cfRule type="expression" dxfId="62" priority="14">
       <formula>$F12&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="74" priority="13">
+    <cfRule type="expression" dxfId="61" priority="13">
       <formula>$F13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="73" priority="8">
+    <cfRule type="expression" dxfId="60" priority="8">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B13">
-    <cfRule type="expression" dxfId="72" priority="7">
+    <cfRule type="expression" dxfId="59" priority="7">
       <formula>$F15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="expression" dxfId="71" priority="4">
+    <cfRule type="expression" dxfId="58" priority="4">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B28">
-    <cfRule type="expression" dxfId="70" priority="2">
+    <cfRule type="expression" dxfId="57" priority="2">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 B23:B26 B28 C2:C30 F2:M30">
-    <cfRule type="expression" dxfId="69" priority="9">
+    <cfRule type="expression" dxfId="56" priority="9">
       <formula>$N2="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="68" priority="11">
+    <cfRule type="expression" dxfId="55" priority="11">
       <formula>$N18="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="12">
+    <cfRule type="expression" dxfId="54" priority="12">
       <formula>$F18&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B28">
-    <cfRule type="expression" dxfId="66" priority="17">
+    <cfRule type="expression" dxfId="53" priority="17">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="18">
+    <cfRule type="expression" dxfId="52" priority="18">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="64" priority="15">
+    <cfRule type="expression" dxfId="51" priority="15">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="16">
+    <cfRule type="expression" dxfId="50" priority="16">
       <formula>#REF!&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="19">
+    <cfRule type="expression" dxfId="49" priority="19">
       <formula>$N29="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="20">
+    <cfRule type="expression" dxfId="48" priority="20">
       <formula>$F29&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="21">
+    <cfRule type="expression" dxfId="47" priority="21">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="22">
+    <cfRule type="expression" dxfId="46" priority="22">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C30 F2:M30 B21 B23:B26 B28">
-    <cfRule type="expression" dxfId="58" priority="10">
+    <cfRule type="expression" dxfId="45" priority="10">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="expression" dxfId="57" priority="1">
+    <cfRule type="expression" dxfId="44" priority="1">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18918,98 +18918,98 @@
     <mergeCell ref="A18:A21"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3 D2:D30">
-    <cfRule type="expression" dxfId="56" priority="3">
+    <cfRule type="expression" dxfId="43" priority="3">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B9">
-    <cfRule type="expression" dxfId="55" priority="5">
+    <cfRule type="expression" dxfId="42" priority="5">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="54" priority="6">
+    <cfRule type="expression" dxfId="41" priority="6">
       <formula>$F4&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="expression" dxfId="53" priority="14">
+    <cfRule type="expression" dxfId="40" priority="14">
       <formula>$F12&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="52" priority="13">
+    <cfRule type="expression" dxfId="39" priority="13">
       <formula>$F13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="51" priority="8">
+    <cfRule type="expression" dxfId="38" priority="8">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B13">
-    <cfRule type="expression" dxfId="50" priority="7">
+    <cfRule type="expression" dxfId="37" priority="7">
       <formula>$F15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="expression" dxfId="49" priority="4">
+    <cfRule type="expression" dxfId="36" priority="4">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B28">
-    <cfRule type="expression" dxfId="48" priority="2">
+    <cfRule type="expression" dxfId="35" priority="2">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 B23:B26 B28 C2:C30 F2:M30">
-    <cfRule type="expression" dxfId="47" priority="9">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>$N2="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="46" priority="11">
+    <cfRule type="expression" dxfId="33" priority="11">
       <formula>$N18="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>$F18&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B28">
-    <cfRule type="expression" dxfId="44" priority="17">
+    <cfRule type="expression" dxfId="31" priority="17">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="18">
+    <cfRule type="expression" dxfId="30" priority="18">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="42" priority="15">
+    <cfRule type="expression" dxfId="29" priority="15">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="16">
+    <cfRule type="expression" dxfId="28" priority="16">
       <formula>#REF!&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="19">
+    <cfRule type="expression" dxfId="27" priority="19">
       <formula>$N29="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="20">
+    <cfRule type="expression" dxfId="26" priority="20">
       <formula>$F29&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="21">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="22">
+    <cfRule type="expression" dxfId="24" priority="22">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C30 F2:M30 B21 B23:B26 B28">
-    <cfRule type="expression" dxfId="36" priority="10">
+    <cfRule type="expression" dxfId="23" priority="10">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="expression" dxfId="35" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20764,98 +20764,98 @@
     <mergeCell ref="A18:A21"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3 D2:D30">
-    <cfRule type="expression" dxfId="34" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B9">
-    <cfRule type="expression" dxfId="33" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="32" priority="6">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>$F4&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="expression" dxfId="31" priority="14">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>$F12&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="30" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>$F13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="29" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B13">
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>$F15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="expression" dxfId="27" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B28">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 B23:B26 B28 C2:C30 F2:M30">
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>$N2="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="24" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>$N18="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>$F18&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B28">
-    <cfRule type="expression" dxfId="22" priority="17">
+    <cfRule type="expression" dxfId="9" priority="17">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="18">
+    <cfRule type="expression" dxfId="8" priority="18">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="20" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="16">
+    <cfRule type="expression" dxfId="6" priority="16">
       <formula>#REF!&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="5" priority="19">
       <formula>$N29="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="4" priority="20">
       <formula>$F29&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="21">
+    <cfRule type="expression" dxfId="3" priority="21">
       <formula>#REF!="Oui"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="22">
+    <cfRule type="expression" dxfId="2" priority="22">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C30 F2:M30 B21 B23:B26 B28">
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20884,17 +20884,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ee72ef8-afb7-4cab-8045-23d1f296c8e3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3823e97-3c8f-42af-9aa3-4a85adc1b986">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF9263497045A640A8CB558901A6A6C8" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="74a64c617853225d9915ce5c2407eb7f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3823e97-3c8f-42af-9aa3-4a85adc1b986" xmlns:ns3="1ee72ef8-afb7-4cab-8045-23d1f296c8e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2245405c225123f82bf2fff4f792a1eb" ns2:_="" ns3:_="">
     <xsd:import namespace="f3823e97-3c8f-42af-9aa3-4a85adc1b986"/>
@@ -21089,6 +21078,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ee72ef8-afb7-4cab-8045-23d1f296c8e3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3823e97-3c8f-42af-9aa3-4a85adc1b986">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B8A56E-0482-4C34-B391-4275AF43D713}">
   <ds:schemaRefs>
@@ -21098,23 +21098,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DD8CA4D-88CF-4FAD-9219-4EDEC6099C12}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1ee72ef8-afb7-4cab-8045-23d1f296c8e3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f3823e97-3c8f-42af-9aa3-4a85adc1b986"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B8A2DB-F0C8-46F4-AC39-BA8B306E6417}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21133,6 +21116,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DD8CA4D-88CF-4FAD-9219-4EDEC6099C12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1ee72ef8-afb7-4cab-8045-23d1f296c8e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f3823e97-3c8f-42af-9aa3-4a85adc1b986"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{16150599-ebb0-4fcf-94a5-6010823c7bd5}" enabled="0" method="" siteId="{16150599-ebb0-4fcf-94a5-6010823c7bd5}" removed="1"/>

</xml_diff>